<commit_message>
rerun performance tests with unstable sorting
</commit_message>
<xml_diff>
--- a/nw/performance/timings.xlsx
+++ b/nw/performance/timings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/djb/repos/xstuff/nw/performance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884ECD1A-6369-5B4F-BB19-421AA98DFBE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6741AE4F-CCBB-BF42-AE83-90F3429DA84C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15980" yWindow="800" windowWidth="16880" windowHeight="11220" xr2:uid="{6D49A1E4-1C2C-0642-8AD8-5F33A3F20B88}"/>
+    <workbookView xWindow="15820" yWindow="800" windowWidth="17040" windowHeight="11760" xr2:uid="{6D49A1E4-1C2C-0642-8AD8-5F33A3F20B88}"/>
   </bookViews>
   <sheets>
     <sheet name="timings" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="14">
   <si>
     <t>Paragraphs</t>
   </si>
@@ -532,7 +532,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="J3" sqref="J3:J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -627,26 +627,26 @@
         <v>1.4651396563307493</v>
       </c>
       <c r="G3" s="9">
-        <v>879.59954400000004</v>
+        <v>880.06517899999994</v>
       </c>
       <c r="H3" s="14">
         <f t="shared" ref="H3:H10" si="1">G3/D3</f>
-        <v>2.2728670387596899</v>
+        <v>2.2740702299741602</v>
       </c>
       <c r="I3" s="10">
         <f t="shared" ref="I3:I10" si="2">G3/E3</f>
-        <v>1.5512971947341785</v>
+        <v>1.5521184073805439</v>
       </c>
       <c r="J3" s="8">
-        <v>563.55830200000003</v>
+        <v>668.51707699999997</v>
       </c>
       <c r="K3" s="14">
         <f>J3/D3</f>
-        <v>1.4562230025839793</v>
+        <v>1.7274343074935399</v>
       </c>
       <c r="L3" s="19">
         <f t="shared" ref="L3:L17" si="3">E3 / J3</f>
-        <v>1.0061231375489523</v>
+        <v>0.84815940610594165</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -671,26 +671,26 @@
         <v>1.6150349247311826</v>
       </c>
       <c r="G4" s="9">
-        <v>1217.815726</v>
+        <v>1220.598821</v>
       </c>
       <c r="H4" s="14">
         <f t="shared" si="1"/>
-        <v>2.6189585505376347</v>
+        <v>2.624943701075269</v>
       </c>
       <c r="I4" s="10">
         <f t="shared" si="2"/>
-        <v>1.6216110936260724</v>
+        <v>1.6253169890503651</v>
       </c>
       <c r="J4" s="8">
-        <v>726.98033699999996</v>
+        <v>641.07298300000002</v>
       </c>
       <c r="K4" s="14">
         <f t="shared" ref="K4:K17" si="5">J4/D4</f>
-        <v>1.5633985741935483</v>
+        <v>1.3786515763440861</v>
       </c>
       <c r="L4" s="19">
         <f t="shared" si="3"/>
-        <v>1.0330282701992806</v>
+        <v>1.1714598180157592</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -715,26 +715,26 @@
         <v>3.4802897562408219</v>
       </c>
       <c r="G5" s="9">
-        <v>11028.701709999999</v>
+        <v>11897.80673</v>
       </c>
       <c r="H5" s="14">
         <f t="shared" si="1"/>
-        <v>8.0974315051395003</v>
+        <v>8.7355409177679881</v>
       </c>
       <c r="I5" s="10">
         <f t="shared" si="2"/>
-        <v>2.3266544087656102</v>
+        <v>2.5100039162266592</v>
       </c>
       <c r="J5" s="8">
-        <v>5477.1520309999996</v>
+        <v>5497.9921039999999</v>
       </c>
       <c r="K5" s="14">
         <f t="shared" si="5"/>
-        <v>4.0214038406754771</v>
+        <v>4.0367049221732749</v>
       </c>
       <c r="L5" s="19">
         <f t="shared" si="3"/>
-        <v>0.86544149608616183</v>
+        <v>0.86216105049539005</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -759,26 +759,26 @@
         <v>4.1730365345384115</v>
       </c>
       <c r="G6" s="9">
-        <v>14859.189037</v>
+        <v>14903.132895000001</v>
       </c>
       <c r="H6" s="14">
         <f t="shared" si="1"/>
-        <v>9.5927624512588761</v>
+        <v>9.6211316300839247</v>
       </c>
       <c r="I6" s="10">
         <f t="shared" si="2"/>
-        <v>2.2987487341325066</v>
+        <v>2.3055469441626011</v>
       </c>
       <c r="J6" s="8">
-        <v>7597.6980510000003</v>
+        <v>6627.10772</v>
       </c>
       <c r="K6" s="14">
         <f t="shared" si="5"/>
-        <v>4.9049051329890254</v>
+        <v>4.2783135700451904</v>
       </c>
       <c r="L6" s="19">
         <f t="shared" si="3"/>
-        <v>0.8507884294176723</v>
+        <v>0.97539286595450114</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -802,27 +802,27 @@
         <f t="shared" si="0"/>
         <v>4.3583722547692307</v>
       </c>
-      <c r="G7" s="7">
-        <v>16415.768952999999</v>
+      <c r="G7" s="9">
+        <v>15031.086153</v>
       </c>
       <c r="H7" s="14">
         <f t="shared" si="1"/>
-        <v>10.102011663384614</v>
+        <v>9.2498991710769225</v>
       </c>
       <c r="I7" s="10">
         <f t="shared" si="2"/>
-        <v>2.3178404855919084</v>
+        <v>2.1223288490227166</v>
       </c>
       <c r="J7" s="8">
-        <v>8834.7071230000001</v>
+        <v>7389.4488970000002</v>
       </c>
       <c r="K7" s="14">
         <f t="shared" si="5"/>
-        <v>5.436742844923077</v>
+        <v>4.5473531673846157</v>
       </c>
       <c r="L7" s="19">
         <f t="shared" si="3"/>
-        <v>0.80165135248932229</v>
+        <v>0.95844155805385212</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -846,27 +846,27 @@
         <f t="shared" si="0"/>
         <v>5.0676750063525677</v>
       </c>
-      <c r="G8" s="7">
-        <v>24060.342683999999</v>
+      <c r="G8" s="9">
+        <v>20598.70709</v>
       </c>
       <c r="H8" s="14">
         <f t="shared" si="1"/>
-        <v>12.737079239809423</v>
+        <v>10.904556426680783</v>
       </c>
       <c r="I8" s="10">
         <f t="shared" si="2"/>
-        <v>2.5133970161549226</v>
+        <v>2.151786847619749</v>
       </c>
       <c r="J8" s="8">
-        <v>11359.344283</v>
+        <v>9962.8605580000003</v>
       </c>
       <c r="K8" s="14">
         <f t="shared" si="5"/>
-        <v>6.0134167723663312</v>
+        <v>5.2741453456855485</v>
       </c>
       <c r="L8" s="19">
         <f t="shared" si="3"/>
-        <v>0.84272805265057216</v>
+        <v>0.96085236075227221</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -890,27 +890,25 @@
         <f t="shared" si="0"/>
         <v>6.4862626289915966</v>
       </c>
-      <c r="G9" s="7">
-        <v>39804.686694000004</v>
-      </c>
-      <c r="H9" s="14">
-        <f t="shared" si="1"/>
-        <v>16.724658274789917</v>
-      </c>
-      <c r="I9" s="10">
-        <f t="shared" si="2"/>
-        <v>2.5784738040109332</v>
+      <c r="G9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="J9" s="8">
-        <v>19368.706547999998</v>
+        <v>17500.605729999999</v>
       </c>
       <c r="K9" s="14">
         <f t="shared" si="5"/>
-        <v>8.138111994957983</v>
+        <v>7.353195684873949</v>
       </c>
       <c r="L9" s="19">
         <f t="shared" si="3"/>
-        <v>0.79702302364604971</v>
+        <v>0.88210118524851766</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -934,27 +932,25 @@
         <f t="shared" si="0"/>
         <v>8.0553210988286974</v>
       </c>
-      <c r="G10" s="7">
-        <v>51227.201954999997</v>
-      </c>
-      <c r="H10" s="14">
-        <f t="shared" si="1"/>
-        <v>18.750805986456808</v>
-      </c>
-      <c r="I10" s="10">
-        <f t="shared" si="2"/>
-        <v>2.3277540096053171</v>
+      <c r="G10" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="J10" s="8">
-        <v>26814.944871</v>
+        <v>26263.275151000002</v>
       </c>
       <c r="K10" s="14">
         <f t="shared" si="5"/>
-        <v>9.8151335545388001</v>
+        <v>9.6132046672767206</v>
       </c>
       <c r="L10" s="19">
         <f t="shared" si="3"/>
-        <v>0.82070417626703462</v>
+        <v>0.837943368276445</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -978,27 +974,25 @@
         <f t="shared" si="0"/>
         <v>9.342964534047919</v>
       </c>
-      <c r="G11" s="7">
-        <v>80368.632253999996</v>
-      </c>
-      <c r="H11" s="14">
-        <f t="shared" ref="H11:H13" si="6">G11/D11</f>
-        <v>25.336895414249685</v>
-      </c>
-      <c r="I11" s="10">
-        <f t="shared" ref="I11:I13" si="7">G11/E11</f>
-        <v>2.7118689492950754</v>
+      <c r="G11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="J11" s="8">
-        <v>35741.626054</v>
+        <v>36265.528225000002</v>
       </c>
       <c r="K11" s="14">
         <f t="shared" si="5"/>
-        <v>11.26785184552333</v>
+        <v>11.433016464375788</v>
       </c>
       <c r="L11" s="19">
         <f t="shared" si="3"/>
-        <v>0.82916998396281194</v>
+        <v>0.81719155772754493</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -1022,27 +1016,25 @@
         <f t="shared" si="0"/>
         <v>9.6993488120905305</v>
       </c>
-      <c r="G12" s="7">
-        <v>81848.078399000005</v>
-      </c>
-      <c r="H12" s="14">
-        <f t="shared" si="6"/>
-        <v>24.374055508933893</v>
-      </c>
-      <c r="I12" s="10">
-        <f t="shared" si="7"/>
-        <v>2.512957929562333</v>
+      <c r="G12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="J12" s="8">
-        <v>41576.454137000001</v>
+        <v>41516.904816000002</v>
       </c>
       <c r="K12" s="14">
         <f t="shared" si="5"/>
-        <v>12.38131451369863</v>
+        <v>12.363580945801072</v>
       </c>
       <c r="L12" s="19">
         <f t="shared" si="3"/>
-        <v>0.78338602911340427</v>
+        <v>0.78450967034632701</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -1066,27 +1058,25 @@
         <f t="shared" si="0"/>
         <v>11.667045730366493</v>
       </c>
-      <c r="G13" s="7">
-        <v>106004.488187</v>
-      </c>
-      <c r="H13" s="14">
-        <f t="shared" si="6"/>
-        <v>27.749866017539265</v>
-      </c>
-      <c r="I13" s="10">
-        <f t="shared" si="7"/>
-        <v>2.3784826646657509</v>
+      <c r="G13" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="J13" s="8">
-        <v>51614.107096</v>
+        <v>54074.672651000001</v>
       </c>
       <c r="K13" s="14">
         <f t="shared" si="5"/>
-        <v>13.511546360209424</v>
+        <v>14.155673468848168</v>
       </c>
       <c r="L13" s="19">
         <f t="shared" si="3"/>
-        <v>0.86348708129553109</v>
+        <v>0.82419573721036299</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -1110,25 +1100,25 @@
         <f t="shared" si="0"/>
         <v>14.271082865608228</v>
       </c>
-      <c r="G14" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="I14" s="10" t="s">
+      <c r="G14" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" s="9" t="s">
         <v>12</v>
       </c>
       <c r="J14" s="8">
-        <v>73093.072516</v>
+        <v>67932.044580999995</v>
       </c>
       <c r="K14" s="14">
         <f t="shared" si="5"/>
-        <v>16.344604766547405</v>
+        <v>15.190528752459748</v>
       </c>
       <c r="L14" s="19">
         <f t="shared" si="3"/>
-        <v>0.87313722598033905</v>
+        <v>0.93947242378230988</v>
       </c>
     </row>
     <row r="15" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1152,25 +1142,25 @@
         <f t="shared" si="0"/>
         <v>18.060926031942881</v>
       </c>
-      <c r="G15" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="I15" s="10" t="s">
+      <c r="G15" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="9" t="s">
         <v>12</v>
       </c>
       <c r="J15" s="7">
-        <v>107409.357842</v>
+        <v>98069.277424999993</v>
       </c>
       <c r="K15" s="14">
         <f t="shared" si="5"/>
-        <v>20.182141646373545</v>
+        <v>18.427147204998121</v>
       </c>
       <c r="L15" s="20">
         <f t="shared" si="3"/>
-        <v>0.89489640635775558</v>
+        <v>0.9801259973135773</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -1194,25 +1184,25 @@
         <f t="shared" si="0"/>
         <v>20.289538670707071</v>
       </c>
-      <c r="G16" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="I16" s="10" t="s">
+      <c r="G16" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" s="9" t="s">
         <v>12</v>
       </c>
       <c r="J16" s="8">
-        <v>135885.32891400001</v>
+        <v>124797.856075</v>
       </c>
       <c r="K16" s="14">
         <f t="shared" si="5"/>
-        <v>22.876317998989901</v>
+        <v>21.009740079966331</v>
       </c>
       <c r="L16" s="19">
         <f t="shared" si="3"/>
-        <v>0.88692326586835135</v>
+        <v>0.96572059404266497</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -1236,25 +1226,25 @@
         <f t="shared" si="0"/>
         <v>21.421107058345289</v>
       </c>
-      <c r="G17" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H17" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="I17" s="10" t="s">
+      <c r="G17" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="9" t="s">
         <v>12</v>
       </c>
       <c r="J17" s="8">
-        <v>147289.67387299999</v>
+        <v>138404.599919</v>
       </c>
       <c r="K17" s="14">
         <f t="shared" si="5"/>
-        <v>23.479941634465167</v>
+        <v>22.063542151920931</v>
       </c>
       <c r="L17" s="19">
         <f t="shared" si="3"/>
-        <v>0.91231517487684866</v>
+        <v>0.97088250430723744</v>
       </c>
     </row>
   </sheetData>

</xml_diff>